<commit_message>
Small update to prep for season 9
</commit_message>
<xml_diff>
--- a/evan_rpdr_s8.xlsx
+++ b/evan_rpdr_s8.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28016"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Dropbox/Research/Drag Race/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11820" yWindow="0" windowWidth="15780" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="1260" yWindow="12160" windowWidth="15780" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -141,6 +149,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -472,12 +485,12 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -524,7 +537,7 @@
         <v>5.666666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -551,7 +564,7 @@
         <v>9.6666666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -578,7 +591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -605,7 +618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -632,7 +645,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -659,7 +672,7 @@
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -686,7 +699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -713,7 +726,7 @@
         <v>6.333333333333333</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -740,7 +753,7 @@
         <v>5.333333333333333</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -767,7 +780,7 @@
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -797,7 +810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -828,7 +841,7 @@
         <v>2.2282903261868228</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <f>AVERAGE(B2:B13)</f>
         <v>6.25</v>
@@ -854,7 +867,7 @@
         <v>5.083333333333333</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F16" t="s">
         <v>23</v>
       </c>
@@ -863,7 +876,7 @@
         <v>0.42410035499998255</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -871,7 +884,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -879,12 +892,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -892,32 +905,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>